<commit_message>
New architecture files on ring buffeinterface for course throttling mechanism.
</commit_message>
<xml_diff>
--- a/casperbsp/testdocuments/ethernetcpuinterface.xlsx
+++ b/casperbsp/testdocuments/ethernetcpuinterface.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CPU Register Interface" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ARP Interface" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="CPU Receive Interface" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="CPU Transmit Interface" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Requirements ATP Matrix" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Device Utilisation Report" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'ARP Interface'!$A$1:$D$12</definedName>
@@ -19,7 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'CPU Register Interface'!$A$1:$E$49</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'CPU Transmit Interface'!$A$1:$D$20</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="346">
   <si>
     <t xml:space="preserve">Register Test Report</t>
   </si>
@@ -343,7 +345,7 @@
     <t xml:space="preserve">gmac_rx_ringbuffer_slot_clear</t>
   </si>
   <si>
-    <t xml:space="preserve">XGMAC_ClearRXSlot()</t>
+    <t xml:space="preserve">XGMAC_RXSlotClear()</t>
   </si>
   <si>
     <t xml:space="preserve">gmac_rx_ringbuffer_slot_status</t>
@@ -358,6 +360,9 @@
     <t xml:space="preserve">XGMAC_GetRXNumberOfSlotsFilled()</t>
   </si>
   <si>
+    <t xml:space="preserve">Test with packets flowing</t>
+  </si>
+  <si>
     <t xml:space="preserve">gmac_rx_data_read_enable</t>
   </si>
   <si>
@@ -388,7 +393,7 @@
     <t xml:space="preserve">gmac_tx_ringbuffer_slot_set</t>
   </si>
   <si>
-    <t xml:space="preserve">XGMAC_SetTXSlot()</t>
+    <t xml:space="preserve">XGMAC_TXSlotSet()</t>
   </si>
   <si>
     <t xml:space="preserve">gmac_tx_ringbuffer_slot_status</t>
@@ -397,6 +402,9 @@
     <t xml:space="preserve">XGMAC_GetTXSlotStatus()</t>
   </si>
   <si>
+    <t xml:space="preserve">82fc18b</t>
+  </si>
+  <si>
     <t xml:space="preserve">gmac_tx_ringbuffer_number_slots_filled</t>
   </si>
   <si>
@@ -428,6 +436,657 @@
   </si>
   <si>
     <t xml:space="preserve">gmac_tx_data_write_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements ATP Matrix/Verification Cross-reference Matrix (VCRM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paragraph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifiation Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass/Meet Req</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1 Design Constraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The firmware shall be developed on the Xilinx VCU1525 development board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[11]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The firmware shall be developed on the Xilinx VCU118 development board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The firmware shall be tested on the Xilinx VCU1525 development board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Xilinx VCU1525 development board shall be housed in a server with 100GbE NIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The server shall be able to operate the VCU1525 and the 100GbE NIC simultaneously</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The server shall interface to the VCU1525 via a 100GbE Mellanox network switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[8]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The firmware top level block diagram shall be as shown in Figure 1 for the 100GbE architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The firmware top level block diagram shall be as shown in Figure 2 for the 40GbE architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2 Firmware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2.1 General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[10]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only IP cores part of a standard Vivado license shall be used for the development of the
+firmware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[121]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kutleng shall provide a complete Vivado project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All firmware/software generated by Kutleng shall conform to the firmware coding standards in
+[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARAO to verify through code review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2.2 100GbE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The MAC present on the VU9P Virtex Ultrascale+ FPGA on the VCU1525 development board
+shall be utilised for this interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[161]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PHY present on the VU9P Virtex Ultrascale+ FPGA on the VCU1525 development
+board shall be utilised for this interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[17]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 100GbE Ethernet Controller mapping shall satisfy the CASPER Ethernet Controller Map
+Standard as specified in Appendix A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See ATP Tab “CPU Register Interface,ARP Interface”. Kutleng added unique RX and TX interface using Ring Buffers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The microblaze shall utilise the AXI-Lite MM I/F to send/receive control messages to/from the
+100GbE functionality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 100GbE Interface shall support the following ethernet communication protocols:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I, T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kutleng provides RAW Ethernet Frame Interface. SARAO to add code for Casper Framework to implement the specific protocols on top of Ethernet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I, D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARAO Responsibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASPER Software stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICMP (ping packets)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGMP (multicasting)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T, A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DHCP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[20]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The microblaze shall utilise the AXI-Lite MM I/F to send/receive control messages to/from the
+partial reconfiguration functionality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed all partial reconfiguration is done through the Server PC and using RTL code. The Microblaze only reads PR_DONE,PR_ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[201]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The microblaze shall utilise the AXI-Lite MM I/F to send/receive control messages to/from
+the PCIe functionality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[21]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There shall be no dropped transmit or receive packets at full baud rate (25.78125Gbits/s x 4
+lanes using 64/66b encoding) for one hour using QSFP1 link to QSFP2 link via the Mellanox
+Ethernet Switch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[22]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There shall be continuous streaming throughput of at least 98Gbps from QSFP1 link to
+QSFP2 link at the application layer, after 64/66 encoding, Ethernet, IP and UDP overheads, for
+jumbo packets of MTU = 9000.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumbo packets consume a lot of BRAM. Using 1522 MTU maximum data rate is 94.93Gbps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[23]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shall be possible to reset the 100GbE transmit and receive interface and resume comms
+within 10s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not controllable by Kutleng, Xilinx &amp; Mellanox IP dependant. It works during testing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shall be possible to perform 100000 consecutive board power up/down cycles and recover
+the 100GbE comms each time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This cannot be tested by Kutleng. Big risk of blowing up the Xilinx boards and the test will be too long to perform.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 100GbE interface shall be routed via the AXI Stream Mux/Demux block - refer to Figure 1 and Figure 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[26]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 100GbE interface shall route all its data via the AXI-Streaming interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[261]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 100GbE interface shall route all its control data via the AXI-Lite Memory Mapped
+interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[27]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following status lines (TBC) from the 100GbE MAC shall be routed via the AXI Lite
+Memory Map interface to the microblaze:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See ATP TABS “CPU Register Interface” for supported registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● transmit total good packets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● transmit total packets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● transmit total good bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● transmit total bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● transmit frame error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● transmit bad frame checksum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● receive total good packets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● receive total packets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● receive total good bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● receive total bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● receive sync error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● receive status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● receive packet bad frame checksum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● receive aligned error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[28]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Local Bus (LB) &lt;-&gt; AXIS block shall ensure that the 100GbE data is aligned.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removed in 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[29]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AXI streaming mux shall determine, by a dynamic priority-based system shown in Figure
+3 below, which data gets transmitted out of the 100GbE interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[30]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 100GbE interface shall perform port filtering in the streaming data app, microblaze and
+the partial reconfiguration controller as specified below:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● Streaming data app – default 7148 (DEC), but dynamically configurable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● Partial reconfiguration controller – default 7145 (DEC), but dynamically configurable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● All other control packets to the Microblaze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2.4 Partial reconfiguration (PR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[45] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shall be possible to reconfigure the FPGA via the 100GbE interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[451]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It shall be possible to reconfigure the FPGA via the 40GbE interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[452]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shall be possible to reconfigure the FPGA via the PCIe interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[453] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shall be possible to trigger a reconfiguration from the host-PC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[46]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The PR Controller shall perform CRC frame checking.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UDP Checksum is used not CRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[461]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The host-PC shall re-transmit a data frame in the event that the frame fails the CRC checksum until the FPGA is configured.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[47] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The microblaze shall monitor the status of the PR Controller via the AXI-LIte MM I/F using status bits PRDONE and PRERROR .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[48]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The time taken to reconfigure the FPGA, which includes DHCP, should not be longer than 10, seconds once the reconfiguration process is initiated from the host-pc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[49] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ICAP shall be clocked at 80.5MHz or greater.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[50] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reconfiguration file shall be binary in format, but additional formats are allowed for learning purposes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[51] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A static partition of the FPGA fabric shall be present at all times.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resides in FLASH Memoery and live during bootup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[511] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The static partition shall include all firmware shown in Figure 1 and Figure 2, except the DSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is wise to split the PCIe based design and the Ethernet based design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[52] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VCU1525 board on power up should store in on-board flash the default configuration image (static partition image).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[53] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A reconfiguration module (RM) shall be uploaded via the ICAP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[54] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The board shall be delivered with the board’s factory default firmware still located in its default flash location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARAO requirement to put a factory image on the board. Kutleng will put the static partition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[56] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The RM shall occupy at least 80% of the FPGA’s resources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I, A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARAO will have more than 80% free space on the FPGA for the RM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[561] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The static partition shall occupy at least 80% of the FPGA’s resources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorrect the static partition must be as small as possible to free the FPGA at the moment it is less than 4% of the total device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[562] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The partial reconfiguration functionality shall be able to support compressed bitstreams.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2.5 PCIe Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[58] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PCIe interface shall look like a virtual Ethernet interface to the firmware using the Virtual Ethernet MAC and AXI streaming Mux/Demux block.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[591] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shall be possible to access data via the 100GbE/40GbE interface and the PCIe interface simultaneously.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed the PCIe design is seperate from the Ethernet design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[592] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shall be possible to send data via the 100GbE/40GbE interface and the PCIe interface simultaneously.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[593] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shall be possible to determine which ethernet interface a packet is transmitted on using the AXI-Streaming signal, T_USER.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[60] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PCIe architecture shall be implemented using the FPGA on chip PCIe PHY.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[61] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PCIe architecture shall implement a method for DMA interrupt coalescing in order to handle packet interrupts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[610] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PCIe bandwidth achieved shall be measured.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3 DOCUMENTATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[62] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kutleng Engineering Technologies shall provide an approved test procedure and results document.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test results will be captured. ATP document present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[63] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kutleng Engineering Technologies shall provide sufficient comments in their source, so that the user can easily understand the source code and suitable documents can be generated from the source.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[64] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kutleng Engineering Technologies shall provide agreed upon block diagrams and documentation explaining the firmware generated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explanation of block diagrams will be put on firmware documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4 INVESTIGATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req[65]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following Comparisons between using partial reconfiguration and standard reconfiguration shall be made for test purposes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This requirement is unreachable as the design is now only partial reconfiguration the Xilinx tools doesnt allow switching off PR and Switching it back on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● Time to compile the design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● Resource usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● Timing Closure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">● Time to upload bitstream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilization (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUTs utilization moderate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF Utilization too high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAM Utilization too high due to ILA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41 URAM used investigate where used </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSP Utilization moderate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMCM utilisation moderate (Will be eliminated on user design)</t>
   </si>
 </sst>
 </file>
@@ -439,11 +1098,12 @@
     <numFmt numFmtId="165" formatCode="YY/MM/DD"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -462,92 +1122,17 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000C0"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -555,9 +1140,17 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,68 +1159,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -679,8 +1221,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -704,64 +1267,25 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -769,31 +1293,75 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -801,106 +1369,101 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF0000C0"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -912,7 +1475,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -920,7 +1483,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000C0"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
@@ -928,7 +1491,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -957,22 +1520,22 @@
   </sheetPr>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -981,7 +1544,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -994,7 +1557,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +1572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
@@ -1020,7 +1583,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="12" t="s">
         <v>12</v>
@@ -1048,7 +1611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
@@ -1063,7 +1626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13"/>
       <c r="B8" s="12" t="s">
         <v>15</v>
@@ -1076,7 +1639,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
@@ -1091,7 +1654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
       <c r="B10" s="12" t="s">
         <v>18</v>
@@ -1104,7 +1667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
@@ -1119,7 +1682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13"/>
       <c r="B12" s="12" t="s">
         <v>21</v>
@@ -1132,7 +1695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
         <v>22</v>
       </c>
@@ -1147,7 +1710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13"/>
       <c r="B14" s="12" t="s">
         <v>24</v>
@@ -1160,7 +1723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
@@ -1175,7 +1738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13"/>
       <c r="B16" s="12" t="s">
         <v>27</v>
@@ -1188,7 +1751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
         <v>28</v>
       </c>
@@ -1203,7 +1766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13"/>
       <c r="B18" s="12" t="s">
         <v>30</v>
@@ -1216,7 +1779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
         <v>31</v>
       </c>
@@ -1231,7 +1794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13"/>
       <c r="B20" s="12" t="s">
         <v>33</v>
@@ -1244,7 +1807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
         <v>34</v>
       </c>
@@ -1259,7 +1822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
       <c r="B22" s="12" t="s">
         <v>36</v>
@@ -1272,7 +1835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
         <v>37</v>
       </c>
@@ -1287,7 +1850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
       <c r="B24" s="12" t="s">
         <v>39</v>
@@ -1300,7 +1863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
         <v>40</v>
       </c>
@@ -1315,7 +1878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13"/>
       <c r="B26" s="12" t="s">
         <v>42</v>
@@ -1328,7 +1891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
         <v>43</v>
       </c>
@@ -1343,7 +1906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
         <v>45</v>
       </c>
@@ -1358,7 +1921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
         <v>47</v>
       </c>
@@ -1373,7 +1936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
         <v>49</v>
       </c>
@@ -1388,7 +1951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
         <v>51</v>
       </c>
@@ -1403,7 +1966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
         <v>53</v>
       </c>
@@ -1418,7 +1981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
         <v>55</v>
       </c>
@@ -1433,7 +1996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
         <v>57</v>
       </c>
@@ -1448,7 +2011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
         <v>59</v>
       </c>
@@ -1463,7 +2026,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
         <v>61</v>
       </c>
@@ -1478,7 +2041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
         <v>63</v>
       </c>
@@ -1493,7 +2056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
         <v>65</v>
       </c>
@@ -1508,7 +2071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
         <v>67</v>
       </c>
@@ -1523,7 +2086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
         <v>69</v>
       </c>
@@ -1538,7 +2101,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
         <v>71</v>
       </c>
@@ -1553,7 +2116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
         <v>73</v>
       </c>
@@ -1568,7 +2131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
         <v>75</v>
       </c>
@@ -1583,7 +2146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
         <v>77</v>
       </c>
@@ -1598,7 +2161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
         <v>79</v>
       </c>
@@ -1613,7 +2176,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
         <v>81</v>
       </c>
@@ -1628,7 +2191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
         <v>83</v>
       </c>
@@ -1643,7 +2206,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
         <v>85</v>
       </c>
@@ -1658,7 +2221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="15"/>
@@ -1685,7 +2248,7 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="8" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
@@ -1700,30 +2263,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1734,8 +2299,9 @@
         <v>0.52774945295206</v>
       </c>
       <c r="D2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>88</v>
       </c>
@@ -1746,8 +2312,11 @@
         <v>4</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
@@ -1756,84 +2325,118 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>89</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D5" s="17"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
         <v>91</v>
       </c>
       <c r="B6" s="16"/>
-      <c r="C6" s="5"/>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
         <v>92</v>
       </c>
       <c r="B7" s="16"/>
-      <c r="C7" s="19"/>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D9" s="17"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
         <v>96</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
         <v>97</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22"/>
+      <c r="E11" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="23"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
+      <c r="E12" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B9:B11"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
@@ -1848,30 +2451,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1882,8 +2487,9 @@
         <v>0.52774945295206</v>
       </c>
       <c r="D2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>99</v>
       </c>
@@ -1894,8 +2500,11 @@
         <v>4</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
@@ -1904,116 +2513,160 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>100</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
         <v>105</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="19"/>
+      <c r="C9" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="D9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22"/>
+      <c r="E14" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="23"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
+      <c r="E15" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B11:B14"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2026,42 +2679,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="26" t="n">
         <v>43764</v>
       </c>
-      <c r="C2" s="25" t="n">
+      <c r="C2" s="27" t="n">
         <v>0.52774945295206</v>
       </c>
-      <c r="D2" s="25"/>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="27"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>99</v>
       </c>
@@ -2072,8 +2728,11 @@
         <v>4</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
@@ -2082,158 +2741,1925 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12"/>
       <c r="B6" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>118</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>122</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22"/>
+      <c r="E19" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="B11:B19"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H106"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="88.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="29" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="29" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="49.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="30"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F30" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36" s="37" customFormat="true" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="H36" s="37" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H40" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H41" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H42" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H43" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H44" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H45" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H46" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H47" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H48" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H49" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H50" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H51" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H52" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="D53" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H53" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H54" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="55" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="D55" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E55" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="H55" s="37" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F56" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="F57" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F59" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F60" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="35" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="35"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F64" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="C65" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="D65" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E65" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="H65" s="37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C67" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F67" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C68" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F68" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="C69" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F69" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C70" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C71" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="D71" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E71" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F71" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C72" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F72" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="C73" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="D73" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E73" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F73" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C74" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E74" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F74" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H74" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C75" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E75" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F75" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C76" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="F76" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="C77" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F77" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="C78" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="F78" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="C79" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="D79" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E79" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="F79" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="80" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="C80" s="38" t="s">
+        <v>289</v>
+      </c>
+      <c r="D80" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E80" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="H80" s="37" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="C81" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E81" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="F81" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="35" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="C86" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E86" s="29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="C87" s="38" t="s">
+        <v>297</v>
+      </c>
+      <c r="D87" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E87" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="H87" s="37" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="88" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="C88" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="D88" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E88" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="H88" s="37" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C89" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="D89" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E89" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="C90" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="D90" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F90" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C91" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="D91" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E91" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="C92" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="C96" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="D96" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E96" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F96" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="C97" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="D97" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E97" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F97" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H97" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C98" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F98" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H98" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="102" s="37" customFormat="true" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="C102" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="D102" s="39"/>
+      <c r="E102" s="39"/>
+      <c r="H102" s="37" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C103" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="D103" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E103" s="29" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C104" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="D104" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E104" s="29" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C105" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="D105" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E105" s="29" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C106" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="D106" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E106" s="29" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A3:E13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>27300</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>1182240</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>2.3091757</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="42" t="n">
+        <v>5412</v>
+      </c>
+      <c r="C5" s="42" t="n">
+        <v>1182240</v>
+      </c>
+      <c r="D5" s="42" t="n">
+        <v>0.4577751</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>14941</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2364480</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.6318937</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="42" t="s">
+        <v>335</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2160</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>9.120371</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>960</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>4.2708335</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>6840</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.0877193</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>832</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2.6442308</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>15.384616</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.8333334</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>3.3333335</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated requirements ATP matrix with latest values
</commit_message>
<xml_diff>
--- a/casperbsp/testdocuments/ethernetcpuinterface.xlsx
+++ b/casperbsp/testdocuments/ethernetcpuinterface.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="349">
   <si>
     <t xml:space="preserve">Register Test Report</t>
   </si>
@@ -654,6 +654,9 @@
   <si>
     <t xml:space="preserve">The microblaze shall utilise the AXI-Lite MM I/F to send/receive control messages to/from
 the PCIe functionality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCIe abstracted over Ethernet (WIP)</t>
   </si>
   <si>
     <t xml:space="preserve">Req[21]</t>
@@ -672,6 +675,9 @@
 jumbo packets of MTU = 9000.</t>
   </si>
   <si>
+    <t xml:space="preserve">Meet Requirement-Jumboframes not supported</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jumbo packets consume a lot of BRAM. Using 1522 MTU maximum data rate is 94.93Gbps</t>
   </si>
   <si>
@@ -937,6 +943,9 @@
   </si>
   <si>
     <t xml:space="preserve">The PCIe interface shall look like a virtual Ethernet interface to the firmware using the Virtual Ethernet MAC and AXI streaming Mux/Demux block.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet Requirement(WIP)</t>
   </si>
   <si>
     <t xml:space="preserve">Req[591] </t>
@@ -1150,7 +1159,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1161,6 +1170,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF58220"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -1268,7 +1283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1437,6 +1452,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1496,7 +1515,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFF58220"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -1520,7 +1539,7 @@
   </sheetPr>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2454,7 +2473,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2682,7 +2701,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2957,8 +2976,8 @@
   </sheetPr>
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2968,7 +2987,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="88.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="29" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="29" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="49.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
@@ -3436,26 +3455,29 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+    <row r="32" s="37" customFormat="true" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="D32" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="E32" s="29" t="s">
+      <c r="D32" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="39" t="s">
         <v>185</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D33" s="29" t="s">
         <v>147</v>
@@ -3469,10 +3491,10 @@
     </row>
     <row r="34" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>147</v>
@@ -3480,16 +3502,19 @@
       <c r="E34" s="29" t="s">
         <v>185</v>
       </c>
+      <c r="F34" s="0" t="s">
+        <v>210</v>
+      </c>
       <c r="H34" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D35" s="29" t="s">
         <v>147</v>
@@ -3501,15 +3526,15 @@
         <v>149</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" s="37" customFormat="true" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="37" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D36" s="39" t="s">
         <v>147</v>
@@ -3518,15 +3543,15 @@
         <v>185</v>
       </c>
       <c r="H36" s="37" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>147</v>
@@ -3540,10 +3565,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D38" s="29" t="s">
         <v>147</v>
@@ -3557,10 +3582,10 @@
     </row>
     <row r="39" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>147</v>
@@ -3574,21 +3599,21 @@
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F40" s="36" t="s">
         <v>149</v>
       </c>
       <c r="H40" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="28" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D41" s="29" t="s">
         <v>147</v>
@@ -3597,12 +3622,12 @@
         <v>185</v>
       </c>
       <c r="H41" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="28" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D42" s="29" t="s">
         <v>147</v>
@@ -3611,12 +3636,12 @@
         <v>185</v>
       </c>
       <c r="H42" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="28" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D43" s="29" t="s">
         <v>147</v>
@@ -3625,12 +3650,12 @@
         <v>185</v>
       </c>
       <c r="H43" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="28" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D44" s="29" t="s">
         <v>147</v>
@@ -3639,12 +3664,12 @@
         <v>185</v>
       </c>
       <c r="H44" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="28" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D45" s="29" t="s">
         <v>147</v>
@@ -3653,12 +3678,12 @@
         <v>185</v>
       </c>
       <c r="H45" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="28" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D46" s="29" t="s">
         <v>147</v>
@@ -3667,12 +3692,12 @@
         <v>185</v>
       </c>
       <c r="H46" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="28" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D47" s="29" t="s">
         <v>147</v>
@@ -3681,12 +3706,12 @@
         <v>185</v>
       </c>
       <c r="H47" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="28" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D48" s="29" t="s">
         <v>147</v>
@@ -3695,12 +3720,12 @@
         <v>185</v>
       </c>
       <c r="H48" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="28" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D49" s="29" t="s">
         <v>147</v>
@@ -3709,12 +3734,12 @@
         <v>185</v>
       </c>
       <c r="H49" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="28" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D50" s="29" t="s">
         <v>147</v>
@@ -3723,12 +3748,12 @@
         <v>185</v>
       </c>
       <c r="H50" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="28" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D51" s="29" t="s">
         <v>147</v>
@@ -3737,12 +3762,12 @@
         <v>185</v>
       </c>
       <c r="H51" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="28" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D52" s="29" t="s">
         <v>147</v>
@@ -3751,12 +3776,12 @@
         <v>185</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="28" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D53" s="29" t="s">
         <v>147</v>
@@ -3765,12 +3790,12 @@
         <v>185</v>
       </c>
       <c r="H53" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="28" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D54" s="29" t="s">
         <v>147</v>
@@ -3779,15 +3804,15 @@
         <v>185</v>
       </c>
       <c r="H54" s="40" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="37" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D55" s="39" t="s">
         <v>147</v>
@@ -3796,15 +3821,15 @@
         <v>185</v>
       </c>
       <c r="H55" s="37" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D56" s="29" t="s">
         <v>147</v>
@@ -3818,10 +3843,10 @@
     </row>
     <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F57" s="36" t="s">
         <v>149</v>
@@ -3829,7 +3854,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="28" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D58" s="29" t="s">
         <v>147</v>
@@ -3843,7 +3868,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="28" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D59" s="29" t="s">
         <v>147</v>
@@ -3857,7 +3882,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="28" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D60" s="29" t="s">
         <v>147</v>
@@ -3871,7 +3896,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="35" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3879,10 +3904,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D64" s="29" t="s">
         <v>147</v>
@@ -3896,10 +3921,10 @@
     </row>
     <row r="65" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="37" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C65" s="38" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D65" s="39" t="s">
         <v>147</v>
@@ -3913,10 +3938,10 @@
     </row>
     <row r="66" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D66" s="29" t="s">
         <v>147</v>
@@ -3927,10 +3952,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D67" s="29" t="s">
         <v>147</v>
@@ -3944,10 +3969,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D68" s="29" t="s">
         <v>147</v>
@@ -3959,15 +3984,15 @@
         <v>149</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D69" s="29" t="s">
         <v>147</v>
@@ -3979,15 +4004,15 @@
         <v>149</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D70" s="29" t="s">
         <v>147</v>
@@ -3998,10 +4023,10 @@
     </row>
     <row r="71" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D71" s="29" t="s">
         <v>147</v>
@@ -4015,10 +4040,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D72" s="29" t="s">
         <v>147</v>
@@ -4032,10 +4057,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D73" s="29" t="s">
         <v>147</v>
@@ -4049,10 +4074,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D74" s="29" t="s">
         <v>147</v>
@@ -4064,15 +4089,15 @@
         <v>149</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D75" s="29" t="s">
         <v>147</v>
@@ -4084,15 +4109,15 @@
         <v>149</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D76" s="29" t="s">
         <v>147</v>
@@ -4106,10 +4131,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D77" s="29" t="s">
         <v>147</v>
@@ -4123,10 +4148,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C78" s="41" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D78" s="29" t="s">
         <v>147</v>
@@ -4138,58 +4163,58 @@
         <v>149</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D79" s="29" t="s">
         <v>147</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F79" s="36" t="s">
         <v>149</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="80" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="37" t="s">
+        <v>290</v>
+      </c>
+      <c r="C80" s="38" t="s">
+        <v>291</v>
+      </c>
+      <c r="D80" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E80" s="39" t="s">
         <v>288</v>
       </c>
-      <c r="C80" s="38" t="s">
-        <v>289</v>
-      </c>
-      <c r="D80" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="E80" s="39" t="s">
-        <v>286</v>
-      </c>
       <c r="H80" s="37" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D81" s="29" t="s">
         <v>147</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F81" s="36" t="s">
         <v>149</v>
@@ -4197,15 +4222,15 @@
     </row>
     <row r="84" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="35" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D86" s="29" t="s">
         <v>147</v>
@@ -4213,13 +4238,16 @@
       <c r="E86" s="29" t="s">
         <v>148</v>
       </c>
+      <c r="F86" s="42" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="87" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="37" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C87" s="38" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D87" s="39" t="s">
         <v>147</v>
@@ -4228,15 +4256,15 @@
         <v>185</v>
       </c>
       <c r="H87" s="37" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="88" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="37" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C88" s="38" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D88" s="39" t="s">
         <v>147</v>
@@ -4245,29 +4273,32 @@
         <v>185</v>
       </c>
       <c r="H88" s="37" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="C89" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="D89" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="E89" s="29" t="s">
+    </row>
+    <row r="89" s="37" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="C89" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="D89" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E89" s="39" t="s">
         <v>185</v>
+      </c>
+      <c r="H89" s="37" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D90" s="29" t="s">
         <v>147</v>
@@ -4279,12 +4310,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D91" s="29" t="s">
         <v>147</v>
@@ -4292,13 +4323,16 @@
       <c r="E91" s="29" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F91" s="42" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D92" s="29" t="s">
         <v>147</v>
@@ -4306,18 +4340,21 @@
       <c r="E92" s="29" t="s">
         <v>185</v>
       </c>
+      <c r="F92" s="42" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="35" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D96" s="29" t="s">
         <v>147</v>
@@ -4329,15 +4366,15 @@
         <v>149</v>
       </c>
       <c r="H96" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C97" s="28" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D97" s="29" t="s">
         <v>147</v>
@@ -4354,10 +4391,10 @@
     </row>
     <row r="98" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C98" s="28" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D98" s="29" t="s">
         <v>147</v>
@@ -4369,69 +4406,69 @@
         <v>149</v>
       </c>
       <c r="H98" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="35" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="102" s="37" customFormat="true" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="37" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C102" s="38" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D102" s="39"/>
       <c r="E102" s="39"/>
       <c r="H102" s="37" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="28" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D103" s="29" t="s">
         <v>147</v>
       </c>
       <c r="E103" s="29" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="28" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D104" s="29" t="s">
         <v>147</v>
       </c>
       <c r="E104" s="29" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="28" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D105" s="29" t="s">
         <v>147</v>
       </c>
       <c r="E105" s="29" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="D106" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E106" s="29" t="s">
         <v>326</v>
-      </c>
-      <c r="D106" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="E106" s="29" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -4472,16 +4509,16 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>143</v>
@@ -4489,7 +4526,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>27300</v>
@@ -4503,25 +4540,25 @@
       <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42" t="s">
-        <v>331</v>
-      </c>
-      <c r="B5" s="42" t="n">
+      <c r="A5" s="43" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" s="43" t="n">
         <v>5412</v>
       </c>
-      <c r="C5" s="42" t="n">
+      <c r="C5" s="43" t="n">
         <v>1182240</v>
       </c>
-      <c r="D5" s="42" t="n">
+      <c r="D5" s="43" t="n">
         <v>0.4577751</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>14941</v>
@@ -4533,12 +4570,12 @@
         <v>0.6318937</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42" t="s">
-        <v>335</v>
+      <c r="A7" s="43" t="s">
+        <v>338</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>197</v>
@@ -4550,12 +4587,12 @@
         <v>9.120371</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>41</v>
@@ -4567,12 +4604,12 @@
         <v>4.2708335</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>6</v>
@@ -4584,12 +4621,12 @@
         <v>0.0877193</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>22</v>
@@ -4603,7 +4640,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>8</v>
@@ -4617,7 +4654,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>15</v>
@@ -4631,7 +4668,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
@@ -4643,7 +4680,7 @@
         <v>3.3333335</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>